<commit_message>
initial commit of day 3 materials
</commit_message>
<xml_diff>
--- a/day2/Template Data Dictionary.xlsx
+++ b/day2/Template Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/data-science-basics-2023/day2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094B016D-0B7A-F441-9535-A098025DA145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220882F2-E700-0A45-8F55-FC7AA405112D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -987,7 +987,7 @@
   <dimension ref="A1:V1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3207,7 +3207,7 @@
   <dimension ref="A1:V999"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7438,7 +7438,7 @@
   <dimension ref="A1:S999"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>